<commit_message>
add one module, rerender
</commit_message>
<xml_diff>
--- a/assessment_schedule.xlsx
+++ b/assessment_schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xinchen/Documents/GitRepo/websites/csc110-spring2025/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xinchen/Documents/GitRepo/websites/csc110/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67756FE4-6780-9C42-B66D-F9F52E225781}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8EA656D-F3D0-8B49-B945-D009DD911E20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15920" yWindow="2720" windowWidth="22480" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1460" yWindow="8500" windowWidth="15160" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -180,9 +180,6 @@
     <t>Programming Project 10</t>
   </si>
   <si>
-    <t>Midterm 3</t>
-  </si>
-  <si>
     <t>Module 13 Programming Problems</t>
   </si>
   <si>
@@ -201,25 +198,28 @@
     <t>Quiz 08</t>
   </si>
   <si>
+    <t>Quiz 10</t>
+  </si>
+  <si>
+    <t>Quiz 11</t>
+  </si>
+  <si>
+    <t>Short Programming Project 12</t>
+  </si>
+  <si>
+    <t>Programming Project 12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final Exam </t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
     <t>Quiz 09</t>
   </si>
   <si>
-    <t>Quiz 10</t>
-  </si>
-  <si>
-    <t>Quiz 11</t>
-  </si>
-  <si>
     <t>Quiz 12</t>
-  </si>
-  <si>
-    <t>Final Exam 2pm Section</t>
-  </si>
-  <si>
-    <t>Final Exam 1pm Section</t>
-  </si>
-  <si>
-    <t>1pm GITT 129B</t>
   </si>
 </sst>
 </file>
@@ -304,13 +304,13 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -333,19 +333,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -565,8 +566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -577,7 +578,7 @@
     <col min="4" max="26" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -591,7 +592,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -599,13 +600,13 @@
         <v>4</v>
       </c>
       <c r="C2" s="2">
-        <v>45672</v>
+        <v>45895</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -613,13 +614,16 @@
         <v>7</v>
       </c>
       <c r="C3" s="2">
-        <v>45679</v>
-      </c>
-      <c r="D3" s="1" t="s">
+        <v>45902</v>
+      </c>
+      <c r="D3" s="12" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E3" s="7"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="12"/>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -627,111 +631,116 @@
         <v>8</v>
       </c>
       <c r="C4" s="2">
-        <v>45680</v>
-      </c>
-      <c r="D4" s="3" t="s">
+        <v>45903</v>
+      </c>
+      <c r="D4" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E4" s="7"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
+      <c r="B5" s="7" t="s">
+        <v>11</v>
       </c>
       <c r="C5" s="2">
-        <v>45685</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>45909</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="7"/>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="2">
-        <v>45685</v>
+        <v>45910</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>11</v>
+      <c r="B7" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="C7" s="2">
-        <v>45686</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
+        <v>45910</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="2">
-        <v>45687</v>
+        <v>45912</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="2">
+        <v>45916</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="7"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="2">
-        <v>45692</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="C10" s="2">
-        <v>45692</v>
+        <v>45917</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>15</v>
+      <c r="B11" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="C11" s="2">
-        <v>45693</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>45917</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -739,55 +748,58 @@
         <v>16</v>
       </c>
       <c r="C12" s="2">
-        <v>45694</v>
+        <v>45919</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="2">
+        <v>45923</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="7"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="2">
-        <v>45699</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
-        <v>13</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>18</v>
-      </c>
       <c r="C14" s="2">
-        <v>45699</v>
+        <v>45924</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="7" t="s">
-        <v>19</v>
+      <c r="B15" s="5" t="s">
+        <v>18</v>
       </c>
       <c r="C15" s="2">
-        <v>45700</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>45924</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -795,41 +807,44 @@
         <v>20</v>
       </c>
       <c r="C16" s="2">
-        <v>45701</v>
+        <v>45926</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" s="7" t="s">
-        <v>21</v>
+      <c r="B17" s="14" t="s">
+        <v>27</v>
       </c>
       <c r="C17" s="2">
-        <v>45707</v>
+        <v>45930</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
+      <c r="E17" s="7"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="5"/>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C18" s="2">
-        <v>45709</v>
+        <v>45931</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -837,218 +852,220 @@
         <v>23</v>
       </c>
       <c r="C19" s="2">
-        <v>45709</v>
+        <v>45931</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="1">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>24</v>
       </c>
       <c r="C20" s="2">
-        <v>45712</v>
+        <v>45933</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
         <v>20</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>25</v>
+      <c r="B21" s="11" t="s">
+        <v>21</v>
       </c>
       <c r="C21" s="2">
-        <v>45713</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>45937</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C22" s="2">
-        <v>45713</v>
+        <v>45940</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" s="7" t="s">
-        <v>27</v>
+      <c r="B23" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="C23" s="2">
-        <v>45714</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="1">
+        <v>45940</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C24" s="2">
-        <v>45715</v>
+        <v>45943</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>29</v>
+      <c r="B25" s="14" t="s">
+        <v>50</v>
       </c>
       <c r="C25" s="2">
-        <v>45720</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>45944</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" s="7"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>25</v>
       </c>
-      <c r="B26" s="7" t="s">
-        <v>30</v>
+      <c r="B26" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="C26" s="2">
-        <v>45720</v>
+        <v>45945</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27">
+    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
         <v>26</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="C27" s="2">
-        <v>45721</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="1">
+        <v>45945</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C28" s="2">
-        <v>45722</v>
+        <v>45947</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="10">
+    <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" s="7" t="s">
-        <v>52</v>
+      <c r="B29" s="14" t="s">
+        <v>51</v>
       </c>
       <c r="C29" s="2">
-        <v>45735</v>
+        <v>45951</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="10">
+    <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C30" s="2">
-        <v>45737</v>
+        <v>45952</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31">
+    <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
         <v>30</v>
       </c>
-      <c r="B31" s="4" t="s">
-        <v>35</v>
+      <c r="B31" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="C31" s="2">
-        <v>45742</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32">
+        <v>45952</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C32" s="2">
-        <v>45744</v>
+        <v>45954</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="1">
+      <c r="A33">
         <v>32</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C33" s="2">
+        <v>45958</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34">
         <v>33</v>
       </c>
-      <c r="C33" s="2">
-        <v>45744</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F33" s="2"/>
-    </row>
-    <row r="34" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="1">
-        <v>33</v>
-      </c>
       <c r="B34" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C34" s="2">
-        <v>45747</v>
+        <v>45959</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>6</v>
@@ -1058,14 +1075,14 @@
       <c r="A35">
         <v>34</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>37</v>
+      <c r="B35" s="11" t="s">
+        <v>35</v>
       </c>
       <c r="C35" s="2">
-        <v>45748</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>6</v>
+        <v>45965</v>
+      </c>
+      <c r="D35" s="11" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1073,38 +1090,38 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C36" s="2">
-        <v>45748</v>
+        <v>45966</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37">
+      <c r="A37" s="1">
         <v>36</v>
       </c>
-      <c r="B37" s="7" t="s">
-        <v>53</v>
+      <c r="B37" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="C37" s="2">
-        <v>45749</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>5</v>
+        <v>45966</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="1">
+      <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C38" s="2">
-        <v>45750</v>
+        <v>45968</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>6</v>
@@ -1118,223 +1135,223 @@
         <v>40</v>
       </c>
       <c r="C39" s="2">
-        <v>45755</v>
+        <v>45973</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="1">
+      <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>41</v>
       </c>
       <c r="C40" s="2">
-        <v>45755</v>
+        <v>45973</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41">
+      <c r="A41" s="1">
         <v>40</v>
       </c>
-      <c r="B41" s="7" t="s">
-        <v>54</v>
+      <c r="B41" s="4" t="s">
+        <v>42</v>
       </c>
       <c r="C41" s="2">
-        <v>45756</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>5</v>
+        <v>45975</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>41</v>
       </c>
-      <c r="B42" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C42" s="9">
-        <v>45757</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>6</v>
+      <c r="B42" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C42" s="2">
+        <v>45979</v>
+      </c>
+      <c r="D42" s="12" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="11">
+      <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C43" s="9">
-        <v>45762</v>
+      <c r="C43" s="2">
+        <v>45980</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H43" s="11"/>
+      <c r="H43" s="10"/>
     </row>
     <row r="44" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="1">
+      <c r="A44">
         <v>43</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C44" s="9">
-        <v>45762</v>
+      <c r="C44" s="2">
+        <v>45980</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="11">
+      <c r="A45">
         <v>44</v>
       </c>
-      <c r="B45" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C45" s="9">
-        <v>45763</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>5</v>
+      <c r="B45" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C45" s="2">
+        <v>45982</v>
+      </c>
+      <c r="D45" s="12" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>45</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B46" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C46" s="2">
+        <v>45986</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
+        <v>46</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C47" s="2">
+        <v>45987</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48">
         <v>47</v>
       </c>
-      <c r="C46" s="9">
-        <v>45769</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="11">
-        <v>46</v>
-      </c>
-      <c r="B47" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="C47" s="9">
-        <v>45770</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="1">
-        <v>47</v>
-      </c>
       <c r="B48" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C48" s="9">
-        <v>45772</v>
+        <v>48</v>
+      </c>
+      <c r="C48" s="2">
+        <v>45987</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="11">
+      <c r="A49">
         <v>48</v>
       </c>
-      <c r="B49" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C49" s="9">
-        <v>45776</v>
-      </c>
-      <c r="D49" s="3" t="s">
+      <c r="B49" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C49" s="2">
+        <v>45992</v>
+      </c>
+      <c r="D49" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="E49" s="10"/>
-      <c r="F49" s="10"/>
     </row>
     <row r="50" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="1">
+      <c r="A50">
         <v>49</v>
       </c>
-      <c r="B50" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C50" s="9">
-        <v>45776</v>
-      </c>
-      <c r="D50" s="3" t="s">
+      <c r="B50" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C50" s="2">
+        <v>45993</v>
+      </c>
+      <c r="D50" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
+        <v>50</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C51" s="2">
+        <v>45996</v>
+      </c>
+      <c r="D51" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="11">
-        <v>50</v>
-      </c>
-      <c r="B51" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="C51" s="9">
-        <v>45777</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="E51" s="9"/>
+      <c r="F51" s="9"/>
     </row>
     <row r="52" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>51</v>
       </c>
-      <c r="B52" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C52" s="9">
-        <v>45779</v>
+      <c r="B52" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C52" s="2">
+        <v>45996</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="11">
+      <c r="A53">
         <v>52</v>
       </c>
-      <c r="B53" s="12" t="s">
+      <c r="B53" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C53" s="2">
+        <v>45999</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C54" s="2">
+        <v>46001</v>
+      </c>
+      <c r="D54" s="11" t="s">
         <v>57</v>
-      </c>
-      <c r="C53" s="9">
-        <v>45786</v>
-      </c>
-      <c r="D53" s="13" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="11">
-        <v>53</v>
-      </c>
-      <c r="B54" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="C54" s="9">
-        <v>45789</v>
-      </c>
-      <c r="D54" s="13" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
add common final exam
</commit_message>
<xml_diff>
--- a/assessment_schedule.xlsx
+++ b/assessment_schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xinchen/Documents/GitRepo/websites/csc110/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8EA656D-F3D0-8B49-B945-D009DD911E20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2337A4A-9838-B54F-A12E-36C8B4A512B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1460" yWindow="8500" windowWidth="15160" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1460" yWindow="2720" windowWidth="15160" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -213,13 +213,13 @@
     <t xml:space="preserve">Final Exam </t>
   </si>
   <si>
-    <t>TBD</t>
-  </si>
-  <si>
     <t>Quiz 09</t>
   </si>
   <si>
     <t>Quiz 12</t>
+  </si>
+  <si>
+    <t>6-8pm</t>
   </si>
 </sst>
 </file>
@@ -229,11 +229,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -333,20 +340,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -567,7 +575,7 @@
   <dimension ref="A1:H1003"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A26" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1048,7 +1056,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C33" s="2">
         <v>45958</v>
@@ -1287,7 +1295,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C50" s="2">
         <v>45993</v>
@@ -1348,10 +1356,10 @@
         <v>56</v>
       </c>
       <c r="C54" s="2">
-        <v>46001</v>
-      </c>
-      <c r="D54" s="11" t="s">
-        <v>57</v>
+        <v>46003</v>
+      </c>
+      <c r="D54" s="15" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
add final exam date'
z

N
:q!
</commit_message>
<xml_diff>
--- a/assessment_schedule.xlsx
+++ b/assessment_schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xinchen/Documents/GitRepo/websites/csc110/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2337A4A-9838-B54F-A12E-36C8B4A512B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{298F0F66-4C16-3543-B6CF-05431898AB6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1460" yWindow="2720" windowWidth="15160" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1460" yWindow="760" windowWidth="15160" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -219,7 +219,7 @@
     <t>Quiz 12</t>
   </si>
   <si>
-    <t>6-8pm</t>
+    <t>6-8pm, MLNG 350</t>
   </si>
 </sst>
 </file>
@@ -574,8 +574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>